<commit_message>
Corrections to ITMO Unique Identifier regular expression
</commit_message>
<xml_diff>
--- a/AEF_files.synfixed/202504251541---Thailand AEF_2023_2024.synfixed.xlsx
+++ b/AEF_files.synfixed/202504251541---Thailand AEF_2023_2024.synfixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unfccc365.sharepoint.com/sites/Mitigation/Paris Agreement Article 6/Article 6.2/03_CARP/consistency/AEF_files.synfixed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88192F29-5464-0645-AA47-9624BF94755B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{88192F29-5464-0645-AA47-9624BF94755B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DA5BC59-5697-1440-80D2-B1DB60239119}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="41580" windowHeight="16920" tabRatio="618" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="41580" windowHeight="16920" tabRatio="618" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="5" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="178">
   <si>
     <t>Table</t>
   </si>
@@ -520,15 +520,6 @@
       </rPr>
       <t> </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Unique identifier of the ITMO as per decision 6/CMA.4, annex I, para. 5. </t>
-  </si>
-  <si>
-    <t>Refers to the first unique identifier of the ITMO block.</t>
-  </si>
-  <si>
-    <t>Refers to the last unique identifier of the ITMO block.</t>
   </si>
   <si>
     <t>Refers to the first unique identifier of the underlying unit block.</t>
@@ -724,6 +715,12 @@
   </si>
   <si>
     <t>Action date specified in date-month-year format</t>
+  </si>
+  <si>
+    <t>Refers to the first unique identifier of the ITMO block as per decision 6/CMA.4, annex I, para. 5.</t>
+  </si>
+  <si>
+    <t>Refers to the last unique identifier of the ITMO block as per decision 6/CMA.4, annex I, para. 5.</t>
   </si>
 </sst>
 </file>
@@ -1702,10 +1699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3F6B9B-E1BC-4D08-AE97-F15181187A83}">
-  <dimension ref="B1:C108"/>
+  <dimension ref="B1:C106"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A31" zoomScale="60" zoomScaleNormal="117" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A47" zoomScale="110" zoomScaleNormal="117" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1721,12 +1718,12 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B1" s="15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B2" s="15" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="19" x14ac:dyDescent="0.25">
@@ -1779,7 +1776,7 @@
         <v>87</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="42" x14ac:dyDescent="0.2">
@@ -1787,7 +1784,7 @@
         <v>88</v>
       </c>
       <c r="C11" s="70" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.2">
@@ -2011,7 +2008,7 @@
     </row>
     <row r="45" spans="2:3" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="75" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C45" s="76" t="s">
         <v>21</v>
@@ -2038,7 +2035,7 @@
         <v>84</v>
       </c>
       <c r="C48" s="70" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="28" x14ac:dyDescent="0.2">
@@ -2049,425 +2046,409 @@
         <v>125</v>
       </c>
     </row>
-    <row r="50" spans="2:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" ht="28" x14ac:dyDescent="0.2">
       <c r="B50" s="69" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C50" s="70" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="28" x14ac:dyDescent="0.2">
       <c r="B51" s="69" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C51" s="70" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="56" x14ac:dyDescent="0.2">
       <c r="B52" s="69" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C52" s="70" t="s">
-        <v>128</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="56" x14ac:dyDescent="0.2">
       <c r="B53" s="69" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C53" s="70" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" ht="56" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B54" s="69" t="s">
-        <v>39</v>
+        <v>102</v>
       </c>
       <c r="C54" s="70" t="s">
-        <v>71</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B55" s="69" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C55" s="70" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B56" s="69" t="s">
-        <v>103</v>
+        <v>28</v>
       </c>
       <c r="C56" s="70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="B57" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="C57" s="70" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" ht="42" x14ac:dyDescent="0.2">
+      <c r="B58" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" s="70" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="B59" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" s="70" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" ht="28" x14ac:dyDescent="0.2">
+      <c r="B60" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C60" s="70" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B57" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="C57" s="70" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="2:3" ht="60" x14ac:dyDescent="0.2">
-      <c r="B58" s="69" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="70" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B59" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="C59" s="70" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="B60" s="69" t="s">
-        <v>131</v>
-      </c>
-      <c r="C60" s="70" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="61" spans="2:3" ht="28" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B61" s="69" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="C61" s="70" t="s">
-        <v>133</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B62" s="69" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C62" s="70" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" ht="70" x14ac:dyDescent="0.2">
       <c r="B63" s="69" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="C63" s="70" t="s">
-        <v>64</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64" spans="2:3" ht="70" x14ac:dyDescent="0.2">
       <c r="B64" s="69" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C64" s="70" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="65" spans="2:3" ht="70" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:3" ht="84" x14ac:dyDescent="0.2">
       <c r="B65" s="69" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="C65" s="70" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" ht="84" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="56" x14ac:dyDescent="0.2">
       <c r="B66" s="69" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C66" s="70" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="2:3" ht="56" x14ac:dyDescent="0.2">
       <c r="B67" s="69" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C67" s="70" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="68" spans="2:3" ht="56" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="42" x14ac:dyDescent="0.2">
       <c r="B68" s="69" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="C68" s="70" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="2:3" ht="42" x14ac:dyDescent="0.2">
       <c r="B69" s="69" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C69" s="70" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B70" s="69" t="s">
-        <v>105</v>
-      </c>
-      <c r="C70" s="70" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="71" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C71" s="72" t="s">
+      <c r="C70" s="72" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="74" spans="2:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="B74" s="14" t="s">
+    <row r="73" spans="2:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B73" s="14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="16" t="s">
+    <row r="75" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C76" s="16" t="s">
+      <c r="C75" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C76" s="70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B77" s="69" t="s">
-        <v>58</v>
+        <v>24</v>
       </c>
       <c r="C77" s="70" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="28" x14ac:dyDescent="0.2">
       <c r="B78" s="69" t="s">
-        <v>24</v>
+        <v>84</v>
       </c>
       <c r="C78" s="70" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" ht="28" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B79" s="69" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="C79" s="70" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" ht="28" x14ac:dyDescent="0.2">
       <c r="B80" s="69" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C80" s="70" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" ht="28" x14ac:dyDescent="0.2">
       <c r="B81" s="69" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="C81" s="70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" ht="56" x14ac:dyDescent="0.2">
+      <c r="B82" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="C82" s="70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" ht="56" x14ac:dyDescent="0.2">
+      <c r="B83" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="C83" s="70" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B84" s="69" t="s">
+        <v>102</v>
+      </c>
+      <c r="C84" s="70" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B82" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="C82" s="70" t="s">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B85" s="69" t="s">
+        <v>103</v>
+      </c>
+      <c r="C85" s="70" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B83" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="C83" s="70" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="84" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B84" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="C84" s="70" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3" ht="56" x14ac:dyDescent="0.2">
-      <c r="B85" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="C85" s="70" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B86" s="69" t="s">
-        <v>102</v>
+        <v>28</v>
       </c>
       <c r="C86" s="70" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" ht="42" x14ac:dyDescent="0.2">
+      <c r="B87" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="C87" s="70" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" ht="42" x14ac:dyDescent="0.2">
+      <c r="B88" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="C88" s="70" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="B89" s="69" t="s">
+        <v>135</v>
+      </c>
+      <c r="C89" s="70" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B87" s="69" t="s">
-        <v>103</v>
-      </c>
-      <c r="C87" s="70" t="s">
+    <row r="90" spans="2:3" ht="28" x14ac:dyDescent="0.2">
+      <c r="B90" s="69" t="s">
+        <v>98</v>
+      </c>
+      <c r="C90" s="70" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B88" s="69" t="s">
-        <v>28</v>
-      </c>
-      <c r="C88" s="70" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="89" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B89" s="69" t="s">
-        <v>96</v>
-      </c>
-      <c r="C89" s="70" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" ht="42" x14ac:dyDescent="0.2">
-      <c r="B90" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="C90" s="70" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B91" s="69" t="s">
-        <v>138</v>
+        <v>40</v>
       </c>
       <c r="C91" s="70" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B92" s="69" t="s">
-        <v>98</v>
-      </c>
-      <c r="C92" s="70" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B93" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="C93" s="70" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="71" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="71" t="s">
         <v>41</v>
       </c>
-      <c r="C94" s="72" t="s">
+      <c r="C92" s="72" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="97" spans="2:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="B97" s="14" t="s">
+    <row r="95" spans="2:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B95" s="14" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="99" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="16" t="s">
+    <row r="97" spans="2:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C99" s="16" t="s">
+      <c r="C97" s="16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:3" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B98" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B99" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B100" s="11" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B101" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B102" s="11" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C102" s="10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" ht="28" x14ac:dyDescent="0.2">
       <c r="B103" s="11" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" ht="28" x14ac:dyDescent="0.2">
       <c r="B104" s="11" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="C104" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B105" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="106" spans="2:3" ht="28" x14ac:dyDescent="0.2">
-      <c r="B106" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C106" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="107" spans="2:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="71" t="s">
+    <row r="105" spans="2:3" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="71" t="s">
         <v>86</v>
       </c>
-      <c r="C107" s="72" t="s">
+      <c r="C105" s="72" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="108" spans="2:3" ht="19" x14ac:dyDescent="0.25">
-      <c r="B108" s="14"/>
+    <row r="106" spans="2:3" ht="19" x14ac:dyDescent="0.25">
+      <c r="B106" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="49" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
     <brk id="39" max="16383" man="1"/>
-    <brk id="72" max="16383" man="1"/>
+    <brk id="71" max="16383" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
@@ -2476,7 +2457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="216" zoomScaleNormal="139" zoomScaleSheetLayoutView="216" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="216" zoomScaleNormal="139" zoomScaleSheetLayoutView="216" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2499,7 +2480,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
@@ -2515,7 +2496,7 @@
         <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
@@ -2531,7 +2512,7 @@
         <v>87</v>
       </c>
       <c r="C8" s="54" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="29" customHeight="1" x14ac:dyDescent="0.2">
@@ -2539,7 +2520,7 @@
         <v>88</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
@@ -2732,20 +2713,20 @@
     </row>
     <row r="8" spans="2:21" ht="98" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C8" s="78">
         <v>45140</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E8" s="86">
         <v>1</v>
       </c>
       <c r="F8" s="24"/>
       <c r="G8" s="79" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>48</v>
@@ -2757,16 +2738,16 @@
         <v>21</v>
       </c>
       <c r="K8" s="24" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L8" s="24" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M8" s="24" t="s">
         <v>49</v>
       </c>
       <c r="N8" s="24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="O8" s="19" t="s">
         <v>21</v>
@@ -2775,13 +2756,13 @@
         <v>21</v>
       </c>
       <c r="Q8" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="R8" s="19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="S8" s="93" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="T8" s="24" t="s">
         <v>21</v>
@@ -3159,7 +3140,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E8" s="98"/>
       <c r="F8" s="98"/>
@@ -3240,25 +3221,25 @@
         <v>9</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E9" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="F9" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>156</v>
-      </c>
       <c r="H9" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K9" s="19"/>
       <c r="L9" s="19" t="s">
@@ -3295,10 +3276,10 @@
       </c>
       <c r="X9" s="19"/>
       <c r="Y9" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Z9" s="24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AA9" s="45"/>
       <c r="AB9" s="24" t="s">
@@ -3315,7 +3296,7 @@
       </c>
       <c r="AF9" s="19"/>
       <c r="AH9" s="19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="2:34" ht="69" customHeight="1" x14ac:dyDescent="0.2">
@@ -3326,25 +3307,25 @@
         <v>9</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E10" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="F10" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>156</v>
-      </c>
       <c r="H10" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
@@ -3381,10 +3362,10 @@
       </c>
       <c r="X10" s="19"/>
       <c r="Y10" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Z10" s="24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AA10" s="45"/>
       <c r="AB10" s="24" t="s">
@@ -3401,36 +3382,36 @@
       </c>
       <c r="AF10" s="19"/>
       <c r="AH10" s="19" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="2:34" ht="70" x14ac:dyDescent="0.2">
       <c r="B11" s="24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C11" s="92" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E11" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>156</v>
-      </c>
       <c r="H11" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="K11" s="88"/>
       <c r="L11" s="19" t="s">
@@ -3467,10 +3448,10 @@
       </c>
       <c r="X11" s="24"/>
       <c r="Y11" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Z11" s="24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AA11" s="24"/>
       <c r="AB11" s="24" t="s">
@@ -3488,36 +3469,36 @@
       <c r="AF11" s="24"/>
       <c r="AG11" s="24"/>
       <c r="AH11" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="2:34" ht="70" x14ac:dyDescent="0.2">
       <c r="B12" s="24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C12" s="92" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E12" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="G12" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>156</v>
-      </c>
       <c r="H12" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K12" s="88"/>
       <c r="L12" s="19" t="s">
@@ -3554,10 +3535,10 @@
       </c>
       <c r="X12" s="24"/>
       <c r="Y12" s="24" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="Z12" s="24" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="AA12" s="24"/>
       <c r="AB12" s="24" t="s">
@@ -3575,7 +3556,7 @@
       <c r="AF12" s="24"/>
       <c r="AG12" s="24"/>
       <c r="AH12" s="10" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="2:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4333,22 +4314,22 @@
         <v>45140</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F11" s="84">
         <v>107551000061</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="I11" s="19" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J11" s="19"/>
       <c r="K11" s="51"/>
@@ -4358,22 +4339,22 @@
         <v>45140</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F12" s="85">
         <v>105553133008</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H12" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>167</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="51"/>

</xml_diff>